<commit_message>
mise à jour des bases
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_aide.xlsx
+++ b/Remote/Commun/dist_aide.xlsx
@@ -1,28 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B656F2FE-5932-4A67-8B8F-D230E3107C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="dist_aide"/>
+    <sheet name="dist_aide" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dist_aide">'dist_aide'!$A$1:$D$9</definedName>
+    <definedName name="dist_aide">dist_aide!$A$1:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Aide</t>
+  </si>
+  <si>
+    <t>Lien</t>
+  </si>
+  <si>
+    <t>Date_lien</t>
+  </si>
+  <si>
+    <t>Nouveauté</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Nouveautés.html</t>
+  </si>
+  <si>
+    <t>Mode d'emploi</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Manuel duct'air version 4x.html</t>
+  </si>
+  <si>
+    <t>A propos</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Apropos.html</t>
+  </si>
+  <si>
+    <t>Fournisseurs</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/fournisseurs.html</t>
+  </si>
+  <si>
+    <t>Coude</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Aide_C.html</t>
+  </si>
+  <si>
+    <t>Vue euro</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Aide_Projection.html</t>
+  </si>
+  <si>
+    <t>Calcul des déports</t>
+  </si>
+  <si>
+    <t>logo ductair</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Apropos.htm</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -47,11 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyProtection="1" applyNumberFormat="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="general"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -59,13 +126,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -103,7 +178,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -137,6 +212,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -171,9 +247,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -346,176 +423,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row outlineLevel="0" r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>N°</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>Aide</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>Lien</t>
-        </is>
-      </c>
-      <c r="D1" s="0" t="inlineStr">
-        <is>
-          <t>Date_lien</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Nouveauté</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Nouveautés.html</t>
-        </is>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Mode d'emploi</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Manuel duct'air version 4x.html</t>
-        </is>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="0">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>A propos</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Apropos.html</t>
-        </is>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Fournisseurs</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/fournisseurs.html</t>
-        </is>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Coude</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Aide_C.html</t>
-        </is>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Vue euro</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Aide_Projection.html</t>
-        </is>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="0">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>Calcul des déports</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Apropos.html</t>
-        </is>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="0">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>logo ductair</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>https://ductair.github.io/ductaironline/Support/Apropos.htm</t>
-        </is>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
       </c>
       <c r="D9" s="1">
         <v>45536</v>

</xml_diff>

<commit_message>
mise à jour aides pdf
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_aide.xlsx
+++ b/Remote/Commun/dist_aide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B656F2FE-5932-4A67-8B8F-D230E3107C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA67EC45-C62C-49EB-A45A-9860535D6AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9765" yWindow="2910" windowWidth="14190" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_aide" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>N°</t>
   </si>
@@ -40,56 +40,67 @@
     <t>Nouveauté</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Nouveautés.html</t>
-  </si>
-  <si>
     <t>Mode d'emploi</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Manuel duct'air version 4x.html</t>
-  </si>
-  <si>
     <t>A propos</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Apropos.html</t>
-  </si>
-  <si>
     <t>Fournisseurs</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/fournisseurs.html</t>
-  </si>
-  <si>
     <t>Coude</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Aide_C.html</t>
-  </si>
-  <si>
     <t>Vue euro</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Aide_Projection.html</t>
-  </si>
-  <si>
     <t>Calcul des déports</t>
   </si>
   <si>
     <t>logo ductair</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/Apropos.htm</t>
+    <t>https://ductair.github.io/ductaironline/Support/Nouveautés 4x.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/MU.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/apropos.dpf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/dournisseurs.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Aide coudes.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Aide_projection.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/menu.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Remote/Commun/ductair.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,16 +123,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,11 +441,12 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -457,11 +472,11 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -469,13 +484,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,13 +512,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,13 +526,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D6" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -525,13 +540,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,13 +554,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -553,16 +568,26 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="1">
-        <v>45536</v>
+        <v>45696</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{28AF15B1-52E5-4FAB-9747-6BE474D06181}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{AFD194F6-8713-4019-BC35-D42330051D64}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{F94A1FCE-C534-430E-A80A-7CB69E705718}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{571AD073-6C48-4E8A-915A-6AB2F8675DB7}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{91B52938-5E23-4FE7-8D5C-9C2EA914289F}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{3721A6B2-6667-42F5-9339-B2EE5F8325F2}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{40886733-4699-4FB3-8940-4EBE023043C5}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{18E0023C-E298-4DF3-9C2E-E01C045B8B3E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mise à jour avant publication
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_aide.xlsx
+++ b/Remote/Commun/dist_aide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA67EC45-C62C-49EB-A45A-9860535D6AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219E1315-B5EB-4772-94F6-C3120BD37574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="2910" windowWidth="14190" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_aide" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="dist_aide">dist_aide!$A$1:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -70,19 +83,19 @@
     <t>https://ductair.github.io/ductaironline/Support/apropos.dpf</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/dournisseurs.pdf</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Support/Aide coudes.pdf</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Support/Aide_projection.pdf</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Support/menu.pdf</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Remote/Commun/ductair.png</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/Aide_transfo_trémie.pdf</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Support/fournisseurs.pdf</t>
   </si>
 </sst>
 </file>
@@ -438,10 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +490,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,7 +504,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,7 +518,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -515,10 +529,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,10 +543,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,10 +557,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,7 +574,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,10 +585,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
-        <v>45696</v>
+        <v>45748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>